<commit_message>
dsa excel and recursion
</commit_message>
<xml_diff>
--- a/dsa_approach_chart.xlsx
+++ b/dsa_approach_chart.xlsx
@@ -390,7 +390,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -405,7 +404,6 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -414,7 +412,6 @@
       <bottom style="thick">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -423,7 +420,6 @@
       <bottom style="thick">
         <color rgb="FFACCCEA"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -432,7 +428,6 @@
       <bottom style="medium">
         <color theme="4" tint="0.399980"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -447,7 +442,6 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -462,7 +456,6 @@
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="double">
@@ -477,7 +470,6 @@
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -486,7 +478,6 @@
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left/>
@@ -497,7 +488,6 @@
       <bottom style="double">
         <color theme="4"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
@@ -971,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.000000"/>
@@ -1035,6 +1025,11 @@
       </c>
       <c r="C5" s="0" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="0" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>